<commit_message>
Code review comments and fix missing code system version on valuesetimporter
Signed-off-by: TimBishop <tabishop@us.ibm.com>
</commit_message>
<xml_diff>
--- a/cohort-evaluator-spark/src/test/resources/fileSystemValueSets/Test.xlsx
+++ b/cohort-evaluator-spark/src/test/resources/fileSystemValueSets/Test.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\8A0610897\git\quality-measure-and-cohort-service\cohort-engine\src\test\resources\fileSystemValueSets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\8A0610897\git\quality-measure-and-cohort-service\cohort-evaluator-spark\src\test\resources\fileSystemValueSets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC6D45A1-B146-4ACF-A246-49C1B20D3F5F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{947C885F-DE44-4896-81C6-0EC13C680308}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2730" yWindow="2730" windowWidth="21600" windowHeight="11505" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="375" yWindow="600" windowWidth="24855" windowHeight="12630" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Value Set Info" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="42">
   <si>
     <t>Value Set Name</t>
   </si>
@@ -140,6 +140,27 @@
   </si>
   <si>
     <t>10901-7</t>
+  </si>
+  <si>
+    <t>2021-09</t>
+  </si>
+  <si>
+    <t>Display for 2021-09</t>
+  </si>
+  <si>
+    <t>10901-8</t>
+  </si>
+  <si>
+    <t>Display for 10901-8</t>
+  </si>
+  <si>
+    <t>LOINC</t>
+  </si>
+  <si>
+    <t>Display for 10901-8 LOINC</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.6.1</t>
   </si>
 </sst>
 </file>
@@ -752,11 +773,11 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="12" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
+      <selection pane="bottomLeft" activeCell="A16" sqref="A16:XFD16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -874,6 +895,66 @@
         <v>25</v>
       </c>
     </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A12:F12" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
   <printOptions horizontalCentered="1" gridLines="1"/>

</xml_diff>

<commit_message>
Index codes in valuesets for faster lookups (#205)
* Index codes in valuesets for faster lookups

Signed-off-by: TimBishop <tabishop@us.ibm.com>

* Add in --nobest to work around toolchain issues

Signed-off-by: TimBishop <tabishop@us.ibm.com>

* Code review comments and fix missing code system version on
valuesetimporter

Signed-off-by: TimBishop <tabishop@us.ibm.com>

* Add missing dependency

Signed-off-by: TimBishop <tabishop@us.ibm.com>

* Fix bad import, code comment

Signed-off-by: TimBishop <tabishop@us.ibm.com>

* removed unneeded test line

Signed-off-by: TimBishop <tabishop@us.ibm.com>

* Tweak checking when no codeSystem is provided

Signed-off-by: TimBishop <tabishop@us.ibm.com>
Signed-off-by: David Kwasny <dkwasny@us.ibm.com>
</commit_message>
<xml_diff>
--- a/cohort-evaluator-spark/src/test/resources/fileSystemValueSets/Test.xlsx
+++ b/cohort-evaluator-spark/src/test/resources/fileSystemValueSets/Test.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\8A0610897\git\quality-measure-and-cohort-service\cohort-engine\src\test\resources\fileSystemValueSets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\8A0610897\git\quality-measure-and-cohort-service\cohort-evaluator-spark\src\test\resources\fileSystemValueSets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC6D45A1-B146-4ACF-A246-49C1B20D3F5F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{947C885F-DE44-4896-81C6-0EC13C680308}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2730" yWindow="2730" windowWidth="21600" windowHeight="11505" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="375" yWindow="600" windowWidth="24855" windowHeight="12630" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Value Set Info" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="42">
   <si>
     <t>Value Set Name</t>
   </si>
@@ -140,6 +140,27 @@
   </si>
   <si>
     <t>10901-7</t>
+  </si>
+  <si>
+    <t>2021-09</t>
+  </si>
+  <si>
+    <t>Display for 2021-09</t>
+  </si>
+  <si>
+    <t>10901-8</t>
+  </si>
+  <si>
+    <t>Display for 10901-8</t>
+  </si>
+  <si>
+    <t>LOINC</t>
+  </si>
+  <si>
+    <t>Display for 10901-8 LOINC</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.6.1</t>
   </si>
 </sst>
 </file>
@@ -752,11 +773,11 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="12" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
+      <selection pane="bottomLeft" activeCell="A16" sqref="A16:XFD16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -874,6 +895,66 @@
         <v>25</v>
       </c>
     </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A12:F12" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
   <printOptions horizontalCentered="1" gridLines="1"/>

</xml_diff>